<commit_message>
updating broken web links
</commit_message>
<xml_diff>
--- a/data/4dsw_eligible_citations_links.xlsx
+++ b/data/4dsw_eligible_citations_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/strevino_uoregon_edu/Documents/Desktop/HEDCO Institute/GitHub R Projects/4DSW_Scoping_Review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="559" documentId="8_{DD2EE4A3-A625-40AE-A745-58941D767F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC4832FE-0F1B-480D-85F1-4546CA8CE809}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="8_{DD2EE4A3-A625-40AE-A745-58941D767F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDE7007B-AF73-4186-9E1B-1883CE2B0269}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,9 +781,6 @@
     <t>A comparative study of transporation costs for a four-day school week and a five day school week for Dougherty County schools</t>
   </si>
   <si>
-    <t>https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=A+comparative+study+of+transporation+costs+for+a+four-day+school+week+and+a+five+day+school+week+for+Dougherty+County+schools&amp;issn=&amp;date=1984-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Palmer%2C+John+D.%2C+Jr.&amp;isbn=978-1-369-36344-9&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/</t>
-  </si>
-  <si>
     <t>Charlton, Colleen A. (1983).  A Study of Colorado's Four-Day School Week Program As It Relates to Utilization of School Facilities #journal#, #volume#(#issue#),  1</t>
   </si>
   <si>
@@ -943,9 +940,6 @@
     <t>https://digitalcommons.lindenwood.edu/cgi/viewcontent.cgi?article=1694&amp;context=dissertations</t>
   </si>
   <si>
-    <t>https://scholarworks.montana.edu/xmlui/bitstream/handle/1/10115/AmysR1216.pdf?sequ</t>
-  </si>
-  <si>
     <t>https://files.eric.ed.gov/fulltext/EJ1225164.pdf</t>
   </si>
   <si>
@@ -1006,9 +1000,6 @@
     <t>https://muse.jhu.edu/pub/34/article/784649/pdf?casa_token=jof4z6ITdwYAAAAA:JG5LnbgriNNEy4bhP-axKvEj0ydm0Clzmw4ACRz_cEysrmsOMrlmbM5eVZxpFNLmgYQuCS7p6g</t>
   </si>
   <si>
-    <t>https://d1wqtxts1xzle7.cloudfront.net/76581555/leiseth-dissertation-casestudy-libre.pdf?1639702028=&amp;response-content-disposition=inline%3B+filename%3DA_Case_Study_of_the_Four_Day_School_Week.pdf&amp;Expires=1696263512&amp;Signature=hGKySDEAGKOsIIaZyv~jGegipmWfQe51vkNtqAkEijc5Le6wmZwI~pwx1w1njd076aCjiYqZhHrmNsQ7BNuU81HhI8-eGwFOb2Q-mgRsKIKx5WPwl9jk7eiWep~IVNYy3lPFNouf59MoXseumgqx~sq2ylP7~w5S3KhRlDwtiPKnld4578sXnY2g9CK09fJZ6h6GWgUOgfRlgp~uDyUutmpN-U-lA3iJwvEuwdWMWsjqj~PnGIMxWsWyhLdINow2XDkIpemDpxgxOpBjZPnFH1qk0w9rhYYmk4vNEpwB6yQSW-4WjHmnUYXnG806sb1SSLvTwt-NkHPbgbGBmma0rA__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA</t>
-  </si>
-  <si>
     <t>https://nwmissouri.edu/library/researchpapers/2014/Knapp,%20Kathryn.pdf</t>
   </si>
   <si>
@@ -1037,9 +1028,6 @@
   </si>
   <si>
     <t>https://bearworks.missouristate.edu/cgi/viewcontent.cgi?article=1160&amp;context=articles-coe</t>
-  </si>
-  <si>
-    <t>https://d1wqtxts1xzle7.cloudfront.net/79387510/s10588-015-9198-5-libre.pdf?1642897275=&amp;response-content-disposition=inline%3B+filename%3DWeekends_as_social_distancing_and_their.pdf&amp;Expires=1696264685&amp;Signature=Wis-HexzH2HsF3YhODAoEtEATzrcgDXLfIJBgaILl4Zdnc5ptuUGQdY14kCFNnRHoovqef9eETekI-ZKJzanwze~AexOB80KsUfVam2zSVC39YrDAuMqEX4wRjcdtBMFmSrSDhkOnLBAo6OI3a3TOhh67RgJPWhASK7q8hVEj1VguNu-NCsHh4oWszUoOz-MuuXkHwJglQD32IGqcuXiHtAHGtEUnuIy1zb8LqtumL05vruqGSCVwmKeZneUd97KgVUvggthIMHG1CsD2UXIByFhyF0DtchiWRwRTQPjANDadwJhYjKuoCaZRusZUYdHiHN~1HF6-a1EfSwR3MYwpw__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA</t>
   </si>
   <si>
     <t>https://files.eric.ed.gov/fulltext/ED497760.pdf</t>
@@ -1274,6 +1262,18 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/abs/pii/S0885200622001387</t>
+  </si>
+  <si>
+    <t>https://www.proquest.com/openview/18eeda1fe30c14c8118424cc30e6e2b8/1?pq-origsite=gscholar&amp;cbl=18750</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10588-015-9198-5</t>
+  </si>
+  <si>
+    <t>https://www.proquest.com/openview/de319bec3de80be3c5c1721f151ab5ad/1?pq-origsite=gscholar&amp;cbl=18750</t>
+  </si>
+  <si>
+    <t>https://troyuniversity.on.worldcat.org/search/detail/719377305?queryString=ti%3A%28%E2%80%A2%09A%20comparative%20study%20of%20transportation%20costs%20for%20a%20four-day%20school%20week%20and%20a%20five%20day%20school%20week%20for%20Dougherty%20County%20schools%29&amp;databaseList=217%2C283%2C285%2C638&amp;origPageViewName=pages%2Fadvanced-search-page&amp;clusterResults=&amp;groupVariantRecords=&amp;expandSearch=true&amp;translateSearch=false&amp;queryTranslationLanguage=&amp;lang=en&amp;scope=wz%3A475</t>
   </si>
 </sst>
 </file>
@@ -1677,8 +1677,8 @@
   <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E113" sqref="E113"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1707,16 +1707,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -1730,7 +1730,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1746,7 +1746,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1762,7 +1762,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1778,7 +1778,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1795,10 +1795,10 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -1813,7 +1813,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -1829,7 +1829,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1848,7 +1848,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1864,10 +1864,10 @@
         <v>22</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H10" s="2"/>
     </row>
@@ -1882,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -1898,7 +1898,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>27</v>
@@ -1916,7 +1916,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1932,7 +1932,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -1948,7 +1948,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1964,7 +1964,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1980,7 +1980,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1996,7 +1996,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -2012,10 +2012,10 @@
         <v>41</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -2030,10 +2030,10 @@
         <v>43</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -2048,7 +2048,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2065,7 +2065,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -2081,10 +2081,10 @@
         <v>49</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -2099,7 +2099,7 @@
         <v>51</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2115,7 +2115,7 @@
         <v>53</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>54</v>
@@ -2133,7 +2133,7 @@
         <v>56</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2152,7 +2152,7 @@
         <v>59</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F27" s="6"/>
       <c r="H27" s="2"/>
@@ -2168,7 +2168,7 @@
         <v>61</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -2202,8 +2202,8 @@
       <c r="C30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>306</v>
+      <c r="E30" s="8" t="s">
+        <v>408</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2235,10 +2235,10 @@
         <v>72</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -2253,10 +2253,10 @@
         <v>74</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -2271,10 +2271,10 @@
         <v>76</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -2289,10 +2289,10 @@
         <v>78</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -2307,7 +2307,7 @@
         <v>80</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2345,7 +2345,7 @@
         <v>87</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -2364,7 +2364,7 @@
         <v>90</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -2402,7 +2402,7 @@
         <v>97</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -2421,7 +2421,7 @@
         <v>100</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F42" s="6"/>
     </row>
@@ -2439,7 +2439,7 @@
         <v>103</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -2474,7 +2474,7 @@
         <v>109</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -2490,7 +2490,7 @@
         <v>111</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -2506,10 +2506,10 @@
         <v>113</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="H47" s="2"/>
     </row>
@@ -2524,7 +2524,7 @@
         <v>115</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -2556,10 +2556,10 @@
         <v>120</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H50" s="2"/>
     </row>
@@ -2574,7 +2574,7 @@
         <v>122</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>123</v>
@@ -2592,10 +2592,10 @@
         <v>125</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H52" s="2"/>
     </row>
@@ -2610,7 +2610,7 @@
         <v>127</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>128</v>
@@ -2628,7 +2628,7 @@
         <v>130</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -2644,7 +2644,7 @@
         <v>132</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>133</v>
@@ -2662,7 +2662,7 @@
         <v>135</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -2678,7 +2678,7 @@
         <v>137</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -2694,7 +2694,7 @@
         <v>139</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -2710,7 +2710,7 @@
         <v>141</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -2742,7 +2742,7 @@
         <v>146</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>147</v>
@@ -2767,7 +2767,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -2781,7 +2781,7 @@
         <v>153</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2800,7 +2800,7 @@
         <v>156</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2816,7 +2816,7 @@
         <v>158</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -2832,10 +2832,10 @@
         <v>160</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
@@ -2849,7 +2849,7 @@
         <v>162</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -2881,7 +2881,7 @@
         <v>167</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -2900,10 +2900,10 @@
         <v>170</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
@@ -2917,7 +2917,7 @@
         <v>172</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -2933,7 +2933,7 @@
         <v>174</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -2949,13 +2949,13 @@
         <v>176</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="299.25" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="63" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>90</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>178</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>327</v>
+        <v>406</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -2982,7 +2982,7 @@
         <v>180</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -3015,7 +3015,7 @@
         <v>185</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -3031,10 +3031,10 @@
         <v>187</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
@@ -3051,7 +3051,7 @@
         <v>190</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -3067,7 +3067,7 @@
         <v>192</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -3083,7 +3083,7 @@
         <v>194</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>195</v>
@@ -3100,7 +3100,7 @@
         <v>197</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -3116,7 +3116,7 @@
         <v>199</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G83" s="6" t="s">
         <v>200</v>
@@ -3133,7 +3133,7 @@
         <v>202</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="G84" s="6" t="s">
         <v>203</v>
@@ -3150,7 +3150,7 @@
         <v>205</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G85" s="6" t="s">
         <v>206</v>
@@ -3167,7 +3167,7 @@
         <v>208</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>209</v>
@@ -3184,7 +3184,7 @@
         <v>211</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G87" s="6" t="s">
         <v>212</v>
@@ -3201,7 +3201,7 @@
         <v>214</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
@@ -3217,7 +3217,7 @@
         <v>216</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>217</v>
@@ -3234,7 +3234,7 @@
         <v>219</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>220</v>
@@ -3251,7 +3251,7 @@
         <v>222</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>223</v>
@@ -3268,7 +3268,7 @@
         <v>225</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
@@ -3284,7 +3284,7 @@
         <v>227</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G93" s="6" t="s">
         <v>228</v>
@@ -3301,7 +3301,7 @@
         <v>230</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -3317,7 +3317,7 @@
         <v>232</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
@@ -3333,12 +3333,12 @@
         <v>234</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" spans="1:7" ht="299.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>489</v>
       </c>
@@ -3351,8 +3351,8 @@
       <c r="D97" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E97" s="4" t="s">
-        <v>338</v>
+      <c r="E97" s="8" t="s">
+        <v>407</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
@@ -3382,7 +3382,7 @@
         <v>242</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
@@ -3398,7 +3398,7 @@
         <v>244</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
@@ -3414,7 +3414,7 @@
         <v>246</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
@@ -3430,13 +3430,13 @@
         <v>248</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="236.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1036</v>
       </c>
@@ -3446,25 +3446,26 @@
       <c r="C103" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="G103" s="2" t="s">
-        <v>252</v>
-      </c>
+      <c r="E103" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="G103" s="2"/>
     </row>
     <row r="104" spans="1:7" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>1049</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="F104" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="G104" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="F104" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="204.75" x14ac:dyDescent="0.25">
@@ -3472,16 +3473,16 @@
         <v>1058</v>
       </c>
       <c r="B105" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="F105" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="G105" s="6" t="s">
         <v>257</v>
-      </c>
-      <c r="F105" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="220.5" x14ac:dyDescent="0.25">
@@ -3489,16 +3490,16 @@
         <v>1059</v>
       </c>
       <c r="B106" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="F106" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="G106" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="G106" s="2" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="94.5" x14ac:dyDescent="0.25">
@@ -3506,13 +3507,13 @@
         <v>1062</v>
       </c>
       <c r="B107" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="E107" s="4" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
@@ -3522,16 +3523,16 @@
         <v>1068</v>
       </c>
       <c r="B108" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="F108" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="G108" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="189" x14ac:dyDescent="0.25">
@@ -3539,16 +3540,16 @@
         <v>2125</v>
       </c>
       <c r="B109" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="F109" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="G109" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="F109" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
@@ -3556,16 +3557,16 @@
         <v>2940</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="D110" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D110" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="E110" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
@@ -3575,16 +3576,16 @@
         <v>2944</v>
       </c>
       <c r="B111" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C111" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="D111" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="E111" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
@@ -3594,16 +3595,16 @@
         <v>3032</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="D112" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="E112" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -3613,16 +3614,16 @@
         <v>3037</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="F113" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -3630,16 +3631,16 @@
         <v>3053</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="F114" s="8" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -3647,13 +3648,13 @@
         <v>3054</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="E115" s="4" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
@@ -3663,16 +3664,16 @@
         <v>3056</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="F116" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H116" s="2"/>
     </row>
@@ -3701,139 +3702,140 @@
     <hyperlink ref="E26" r:id="rId17" xr:uid="{8F23CDCB-02D0-4AFB-9021-6D55E33040CB}"/>
     <hyperlink ref="E28" r:id="rId18" xr:uid="{C283E0D2-1D6F-439D-85B0-936881E72830}"/>
     <hyperlink ref="E29" r:id="rId19" xr:uid="{7AC187CB-4836-401E-B864-863209FA6E32}"/>
-    <hyperlink ref="E30" r:id="rId20" xr:uid="{BB9B0F28-219B-47A8-BC4B-65537D1A7726}"/>
-    <hyperlink ref="E31" r:id="rId21" xr:uid="{25EDA559-2CEF-4E44-8A06-E546F2B84006}"/>
-    <hyperlink ref="E36" r:id="rId22" xr:uid="{8FD33C4B-1CE3-46B3-A345-C21880F1752B}"/>
-    <hyperlink ref="E37" r:id="rId23" xr:uid="{93933E02-1ADB-4833-B0BF-E76973463EFD}"/>
-    <hyperlink ref="E38" r:id="rId24" xr:uid="{D4C64ECE-73E4-4CA3-AB45-13D807C4BCD1}"/>
-    <hyperlink ref="E39" r:id="rId25" xr:uid="{726B6699-D227-4F54-9DF6-317184A039DA}"/>
-    <hyperlink ref="E40" r:id="rId26" xr:uid="{79F1D1C5-D2E3-4FB6-8A42-30B6AAEEF86B}"/>
-    <hyperlink ref="E41" r:id="rId27" xr:uid="{20E8E01D-78AA-47AC-9647-41ACA9F319CB}"/>
-    <hyperlink ref="E43" r:id="rId28" xr:uid="{6A1DBB6C-24C8-41BD-A533-0EA7030055CA}"/>
-    <hyperlink ref="E44" r:id="rId29" xr:uid="{38840935-F564-4B2F-AF98-2373338AD887}"/>
-    <hyperlink ref="E45" r:id="rId30" xr:uid="{7D0E3DAE-672A-426E-ACAC-FAE418B4A88B}"/>
-    <hyperlink ref="E46" r:id="rId31" xr:uid="{B9916AA6-CF01-4BC3-BCC9-F57517EFCE1E}"/>
-    <hyperlink ref="E48" r:id="rId32" display="https://www.researchgate.net/profile/Kenneth_David_Strang/publication/318759251_Compressed_school_week_cultural_bias_against_English_Second_Language_student_performance_on_standardized_exams/links/597beb0a0f7e9b8802a94eae/Compressed-school-week-cultural-bias-against-English-Second-Language-student-performance-on-standardized-exams.pdf" xr:uid="{7FB4992C-4B4C-43CD-B296-8FFB935B2BF6}"/>
-    <hyperlink ref="E49" r:id="rId33" xr:uid="{9F240B81-948D-4D36-A688-55516C839E5B}"/>
-    <hyperlink ref="E54" r:id="rId34" xr:uid="{AFB2864A-A3BE-41C4-B7A2-577848D39FDF}"/>
-    <hyperlink ref="E56" r:id="rId35" xr:uid="{55D8ECA8-7BB8-43B4-8508-68F0B8B1327A}"/>
-    <hyperlink ref="E57" r:id="rId36" xr:uid="{403C5BB8-0295-4B17-A4BE-A7B60248A0E6}"/>
-    <hyperlink ref="E58" r:id="rId37" xr:uid="{4FF8993C-AF6D-4835-98AE-76B962E123C7}"/>
-    <hyperlink ref="E59" r:id="rId38" xr:uid="{ABC7321F-2557-486C-814E-68916EB62DAE}"/>
-    <hyperlink ref="E60" r:id="rId39" xr:uid="{0DDA3743-0C6A-4669-904F-B50DB4671549}"/>
-    <hyperlink ref="E62" r:id="rId40" xr:uid="{FBE4A921-F47C-49B4-920A-66482F71D76C}"/>
-    <hyperlink ref="E63" r:id="rId41" xr:uid="{EB5B1EAB-5BAD-4F14-8508-F98623DA2E55}"/>
-    <hyperlink ref="E65" r:id="rId42" xr:uid="{19EDA5A9-D350-4878-8439-07D4C5D87CA9}"/>
-    <hyperlink ref="E67" r:id="rId43" xr:uid="{29CAADCE-6EA2-4A75-A855-EA8C417DFC2E}"/>
-    <hyperlink ref="E68" r:id="rId44" xr:uid="{0FFE9A48-9BF4-450F-8C41-448EA45A1037}"/>
-    <hyperlink ref="E69" r:id="rId45" xr:uid="{7B403720-5732-4579-A81A-460233994424}"/>
-    <hyperlink ref="E71" r:id="rId46" xr:uid="{6E10ACEA-B39A-4D9B-B860-BC22E689266B}"/>
-    <hyperlink ref="E72" r:id="rId47" xr:uid="{B6653391-ACA1-49A5-B4A7-0383B0336B36}"/>
-    <hyperlink ref="E74" r:id="rId48" display="https://d1wqtxts1xzle7.cloudfront.net/76581555/leiseth-dissertation-casestudy-libre.pdf?1639702028=&amp;response-content-disposition=inline%3B+filename%3DA_Case_Study_of_the_Four_Day_School_Week.pdf&amp;Expires=1696263512&amp;Signature=hGKySDEAGKOsIIaZyv~jGegipmWfQe51vkNtqAkEijc5Le6wmZwI~pwx1w1njd076aCjiYqZhHrmNsQ7BNuU81HhI8-eGwFOb2Q-mgRsKIKx5WPwl9jk7eiWep~IVNYy3lPFNouf59MoXseumgqx~sq2ylP7~w5S3KhRlDwtiPKnld4578sXnY2g9CK09fJZ6h6GWgUOgfRlgp~uDyUutmpN-U-lA3iJwvEuwdWMWsjqj~PnGIMxWsWyhLdINow2XDkIpemDpxgxOpBjZPnFH1qk0w9rhYYmk4vNEpwB6yQSW-4WjHmnUYXnG806sb1SSLvTwt-NkHPbgbGBmma0rA__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA" xr:uid="{22910DB3-7BB1-4EA3-BFA9-B800FCDC40CB}"/>
-    <hyperlink ref="E75" r:id="rId49" xr:uid="{B93D594A-EBBD-435A-ABC8-033AA4A45C28}"/>
-    <hyperlink ref="G76" r:id="rId50" xr:uid="{EE0BFC8C-3D01-42C2-BAEB-B237BABF1A69}"/>
-    <hyperlink ref="E77" r:id="rId51" xr:uid="{3F6F9499-A97E-4D52-B3A3-0FC835000504}"/>
-    <hyperlink ref="E79" r:id="rId52" xr:uid="{29055D43-0525-4622-B58C-20DC934FBDC6}"/>
-    <hyperlink ref="E80" r:id="rId53" xr:uid="{9809B794-EB38-4209-AEE7-7CD866741154}"/>
-    <hyperlink ref="E82" r:id="rId54" xr:uid="{CFE5B0D6-A49F-46D0-AE67-5AF70E374F92}"/>
-    <hyperlink ref="E88" r:id="rId55" xr:uid="{E33C5101-8016-4004-97FF-0229DF5D2814}"/>
-    <hyperlink ref="E92" r:id="rId56" location="main" xr:uid="{62C8B0B9-4840-49B2-834E-11D0CF4C253A}"/>
-    <hyperlink ref="E94" r:id="rId57" xr:uid="{3CA66FC6-9EAD-4A9D-B0D5-89C0D376292D}"/>
-    <hyperlink ref="E95" r:id="rId58" xr:uid="{82B11CD5-828F-4A24-AB3F-193982E7E8F8}"/>
-    <hyperlink ref="E96" r:id="rId59" xr:uid="{09D59EDF-991D-4D4A-B2CC-A500EB72581A}"/>
-    <hyperlink ref="E97" r:id="rId60" display="https://d1wqtxts1xzle7.cloudfront.net/79387510/s10588-015-9198-5-libre.pdf?1642897275=&amp;response-content-disposition=inline%3B+filename%3DWeekends_as_social_distancing_and_their.pdf&amp;Expires=1696264685&amp;Signature=Wis-HexzH2HsF3YhODAoEtEATzrcgDXLfIJBgaILl4Zdnc5ptuUGQdY14kCFNnRHoovqef9eETekI-ZKJzanwze~AexOB80KsUfVam2zSVC39YrDAuMqEX4wRjcdtBMFmSrSDhkOnLBAo6OI3a3TOhh67RgJPWhASK7q8hVEj1VguNu-NCsHh4oWszUoOz-MuuXkHwJglQD32IGqcuXiHtAHGtEUnuIy1zb8LqtumL05vruqGSCVwmKeZneUd97KgVUvggthIMHG1CsD2UXIByFhyF0DtchiWRwRTQPjANDadwJhYjKuoCaZRusZUYdHiHN~1HF6-a1EfSwR3MYwpw__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA" xr:uid="{1A160E3F-C17B-4DB5-B0AB-645A9C0DA5B2}"/>
-    <hyperlink ref="E99" r:id="rId61" xr:uid="{7D9732F8-4B86-4CC0-BA46-9476AC4FED46}"/>
-    <hyperlink ref="E100" r:id="rId62" xr:uid="{4237288E-4FBF-4F0F-A678-3D2F910795B5}"/>
-    <hyperlink ref="E101" r:id="rId63" xr:uid="{7E5142FC-179E-40DE-9659-9A2FF9FBE683}"/>
-    <hyperlink ref="E107" r:id="rId64" xr:uid="{7B23BB16-71A0-48CE-805C-BFB42298FBE0}"/>
-    <hyperlink ref="E110" r:id="rId65" xr:uid="{4F277C05-BFBA-449F-8752-0E307436EF8B}"/>
-    <hyperlink ref="E111" r:id="rId66" xr:uid="{1BD26E75-488F-4E14-868C-15F5076003C8}"/>
-    <hyperlink ref="E112" r:id="rId67" xr:uid="{82B04AC4-0EEA-4F80-9B1C-210DE51E94D2}"/>
-    <hyperlink ref="E115" r:id="rId68" xr:uid="{AAA3C322-12A9-4415-922C-74D81FBD97D0}"/>
-    <hyperlink ref="G35" r:id="rId69" xr:uid="{37DEB6BB-AE21-4D65-82EC-6C9DBF9BF72E}"/>
-    <hyperlink ref="G47" r:id="rId70" xr:uid="{9CB66888-A383-4365-8DD1-455302DF0674}"/>
-    <hyperlink ref="G19" r:id="rId71" xr:uid="{711B05F0-8104-4514-A551-999C459B0406}"/>
-    <hyperlink ref="G20" r:id="rId72" xr:uid="{86C3D1CA-AFBE-4DEA-B627-F3EE69FC817E}"/>
-    <hyperlink ref="G23" r:id="rId73" xr:uid="{25A09BFF-36CF-4D51-A291-6A60A992586B}"/>
-    <hyperlink ref="G10" r:id="rId74" xr:uid="{DB27E19D-8146-406B-B6BF-26A5F14B3B99}"/>
-    <hyperlink ref="G33" r:id="rId75" xr:uid="{E07246F3-7066-4F69-A65F-98254F580ED2}"/>
-    <hyperlink ref="G32" r:id="rId76" xr:uid="{897C07DD-A940-4F52-BC65-355F4C7ED66F}"/>
-    <hyperlink ref="G66" r:id="rId77" xr:uid="{E00F78D5-8C8F-4AC0-A5D3-3FB528B3DEDC}"/>
-    <hyperlink ref="G70" r:id="rId78" xr:uid="{A052380E-5C98-42C1-A932-5875FDD6FE6B}"/>
-    <hyperlink ref="G73" r:id="rId79" xr:uid="{D5AD41E6-31BC-4E7C-B124-CA962E91B529}"/>
-    <hyperlink ref="G78" r:id="rId80" xr:uid="{1B103026-3767-4018-A1DF-7926BB7E5E25}"/>
-    <hyperlink ref="E64" r:id="rId81" xr:uid="{6FBC4659-CC58-4CDB-A278-79E1B49004ED}"/>
-    <hyperlink ref="G114" r:id="rId82" xr:uid="{46369FA8-2E83-4232-8E12-11FB6447F57B}"/>
-    <hyperlink ref="G113" r:id="rId83" xr:uid="{0C747466-E2A8-4064-9664-38F8692D95BE}"/>
-    <hyperlink ref="G52" r:id="rId84" xr:uid="{79A57BCB-B8A3-42ED-81D1-697677848967}"/>
-    <hyperlink ref="G50" r:id="rId85" xr:uid="{103E2B00-BE99-4D64-A40E-B74E114EFDDE}"/>
-    <hyperlink ref="G34" r:id="rId86" xr:uid="{CB043E3A-3A12-403C-A0EE-125259BC7972}"/>
-    <hyperlink ref="G6" r:id="rId87" xr:uid="{241256EE-D80C-425A-9E44-65827416D99C}"/>
-    <hyperlink ref="E27" r:id="rId88" xr:uid="{1E13DD51-B7EB-4EFC-A0A9-D847FE9069E7}"/>
-    <hyperlink ref="G55" r:id="rId89" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Impact+of+a+Four-Day+School+Week+on+Student+Discipline+and+Attendance+in+Missouri%3A+A+Quantitative+Study&amp;issn=&amp;date=2021-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Rowden%2C+Angelina&amp;isbn=9798492723514&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{38DBFA6E-C515-4D3D-87CC-444C2A425398}"/>
-    <hyperlink ref="G81" r:id="rId90" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Scheduling+adolescent+achievement%3A+Eighth-graders+and+the+four-day+school+week&amp;issn=&amp;date=2016-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Hegwood%2C+Jessica+Fleming&amp;isbn=978-1-369-48263-8&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{0613F951-D1AE-4EC3-9833-FA8C4694221E}"/>
-    <hyperlink ref="G83" r:id="rId91" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Elementary+Teachers%27+Perceptions+of+Appropriate+Collaborative+Planning+and+Professional+Planning+Time%3A+A+Case+Study&amp;issn=&amp;date=2017-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Wise%2C+Kristi&amp;isbn=978-0-355-10267-3&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{14A9FBBA-105C-4B03-9ABF-4E2F2F55564C}"/>
-    <hyperlink ref="G84" r:id="rId92" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=How+Teachers+Feel+Missouri+School+Schedules+Affect+Teachers+Morale%3A+A+Qualitative+Descriptive+Case+Study&amp;issn=&amp;date=2021-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Smith%2C+Tanya&amp;isbn=979-8-209-99102-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{D4DF9A4B-640B-439E-8775-F74D9F97A2DC}"/>
-    <hyperlink ref="G85" r:id="rId93" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=The+four-day+school+calendar%3A+A+comparative+study+of+student+performance+indicators+in+a+Colorado+school+district&amp;issn=&amp;date=2014-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Reeves%2C+Cheryl+L.&amp;isbn=978-1-303-87204-4&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{5226B787-9144-4A5E-9FBA-10DA9A3B75F6}"/>
-    <hyperlink ref="G87" r:id="rId94" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=The+effect+of+widespread+teacher+furlough+implementation+on+student+performance+on+the+reading%2C+mathematics%2C+and+science+portions+of+the+Hawaiii+State+Assessment&amp;issn=&amp;date=2014-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Lemmer%2C+Bridina+Marie&amp;isbn=978-1-321-05010-3&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{A5E16556-D2D1-4118-90B8-1FEC9124EC80}"/>
-    <hyperlink ref="G89" r:id="rId95" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Explorations+of+Student+and+Parent+Perceptions+of+Changes+in+Traditional+School+Schedule+and+Curriculum+to+Enhance+Competitiveness+with+Charter+Schools&amp;issn=&amp;date=2010-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Kelly%2C+Tiffany+K.&amp;isbn=978-1-124-37958-6&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{A20ED369-9206-4906-B16F-133E337B24F8}"/>
-    <hyperlink ref="G61" r:id="rId96" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Multicase+Exploration+of+Teachers%E2%80%99+Perceptions+of+Experience+of+Working+in+a+4-Day+Work+Week+School+System+Compared+to+a+5-Day+Work+Week+School+System&amp;issn=&amp;date=2020-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Reyes%2C+Lyscelle+M.&amp;isbn=9798698539339&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{19366349-0389-4EB5-BFAA-5FC19CEFC271}"/>
-    <hyperlink ref="G102" r:id="rId97" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=A+COMPARATIVE+CASE+STUDY+OF+THREE+MINNESOTA+SCHOOL+DISTRICTS+EMPLOYING+THE+FOUR-DAY-WEEK+DURING+1982-1983&amp;issn=&amp;date=1985-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=GUSHWA%2C+PRUDENCE+JOANNE&amp;isbn=979-8-205-15586-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{22F43609-39E4-4E93-A3FE-7092A4189348}"/>
-    <hyperlink ref="G91" r:id="rId98" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=A+Quasi-Experimental+Study+Comparing+Work-Life+Balance+and+Turnover+Intentions+Among+Rural+Oklahoma+Classroom+Teachers+Working+Four-Day+and+Five-Day+School+Weeks&amp;issn=&amp;date=2023-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Farber%2C+Misty+Dawn&amp;isbn=9798379420468&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{F99BA589-6518-4F6C-8F80-7D891CE3643F}"/>
-    <hyperlink ref="G93" r:id="rId99" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=The+Four-Day+School+Week+as+a+Path+for+Principal+Attraction+and+Retention%3A+Perceptions+of+Elementary+Principals+in+Missouri&amp;issn=&amp;date=2022-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Weber%2C+Laura+Elizabeth&amp;isbn=9798371990358&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{080115B2-EE11-4BBB-9C85-4C7B4A1AB587}"/>
-    <hyperlink ref="G25" r:id="rId100" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Can+the+4-day+school+week+work%3A+An+analysis+of+the+impact+of+the+4-day+school+week+on+a+rural+Georgia+school+district&amp;issn=&amp;date=2011-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Bell%2C+Jeffrey+L.&amp;isbn=978-1-124-72727-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{6C849674-A5F1-4DB7-97F2-46FD9340B54D}"/>
-    <hyperlink ref="G53" r:id="rId101" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=A+Case+Study+of+the+Influence+of+the+Four-Day+School+Week+on+an+Arizona+School+District&amp;issn=&amp;date=2018-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Savage%2C+Rachel+Marie&amp;isbn=978-0-355-82962-4&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{B6C75ECC-C9F1-43F9-B04E-41908ACC4FFD}"/>
-    <hyperlink ref="G51" r:id="rId102" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Impact+of+a+Four-Day+School+Week+on+Teacher+Preparation&amp;issn=&amp;date=2019-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Schultz%2C+Shawn+C.&amp;isbn=9798662399600&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{0ADED006-B3E9-4FB5-8E8A-C756268CB195}"/>
-    <hyperlink ref="G90" r:id="rId103" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Students%27+Scores+and+Attendance%3A+A+Study+of+South+Dakota+Schools+with+Four-Day+Schedules&amp;issn=&amp;date=2018-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Dolezal%2C+Dennis+W.&amp;isbn=978-0-355-97001-2&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{1543DFBB-C869-4A54-8C15-B482BC5DB0EA}"/>
-    <hyperlink ref="G105" r:id="rId104" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:book&amp;genre=report&amp;sid=ProQ:ProQ%3Aeric&amp;atitle=&amp;title=Colorado%27s+Alternative+School+Calendar+Program+and+the+Four+Day+Week&amp;issn=&amp;date=1982-01-01&amp;volume=&amp;issue=&amp;spage=1&amp;au=Brubacher%2C+Roy+G.%3BStiverson%2C+C.+L.&amp;isbn=&amp;jtitle=&amp;btitle=Colorado%27s+Alternative+School+Calendar+Program+and+the+Four+Day+Week&amp;rft_id=info:eric/ED214719&amp;rft_id=info:doi/" xr:uid="{6F06FFCC-824A-40D9-A384-F16940E98EDB}"/>
-    <hyperlink ref="G109" r:id="rId105" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:journal&amp;genre=article&amp;sid=ProQ:ProQ%3Aeric&amp;atitle=Changing+the+School+Calendar+to+Effect+Energy+Savings&amp;title=School+Business+Affairs&amp;issn=&amp;date=1980-01-01&amp;volume=46&amp;issue=1&amp;spage=11&amp;au=Webb%2C+L.+Dean%3BAshby%2C+Glenn+H.&amp;isbn=&amp;jtitle=School+Business+Affairs&amp;btitle=&amp;rft_id=info:eric/EJ214271&amp;rft_id=info:doi/" xr:uid="{1DBAFCB4-F00A-416F-88E4-8973143D463B}"/>
-    <hyperlink ref="G98" r:id="rId106" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=Investigation+of+the+four-day+school+week&amp;issn=&amp;date=2010-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Bronson%2C+Elizabeth+L.&amp;isbn=979-8-209-73276-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{5DDB6C57-84FC-4BC3-AB9B-5533118D109F}"/>
-    <hyperlink ref="G12" r:id="rId107" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=The+four-day+school+week%3A+Teacher+perceptions+in+a+rural%2Fsecondary+setting&amp;issn=&amp;date=2013-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Farris%2C+Brandon&amp;isbn=978-1-303-13374-9&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{C7A612FE-CED7-4984-B813-1D91DF15C00F}"/>
-    <hyperlink ref="G116" r:id="rId108" xr:uid="{C3FFAE78-7C53-4025-9DF8-CAB3F0011CBB}"/>
-    <hyperlink ref="E2" r:id="rId109" xr:uid="{09C3CA8A-8BC2-4AD9-B08C-84D514554E65}"/>
-    <hyperlink ref="E42" r:id="rId110" xr:uid="{BF57E8F0-8379-4844-A2C0-F3339AC66230}"/>
-    <hyperlink ref="F6" r:id="rId111" xr:uid="{4F06BD45-FC94-4C44-A215-69F3313C6F3F}"/>
-    <hyperlink ref="F10" r:id="rId112" xr:uid="{A13FFFD4-5A08-4BF7-BA9B-D46FA8324C1C}"/>
-    <hyperlink ref="F12" r:id="rId113" xr:uid="{1BF1EA1D-43D8-476D-8BAF-0D9476A35A08}"/>
-    <hyperlink ref="F19" r:id="rId114" xr:uid="{B23139D9-52FE-4A2D-B41C-6AEDA6C1E6BB}"/>
-    <hyperlink ref="F20" r:id="rId115" xr:uid="{945210BB-F866-4ADB-B638-6CA4F832B0A6}"/>
-    <hyperlink ref="F23" r:id="rId116" xr:uid="{08E25523-8C97-448B-96F4-B0C84E945DB7}"/>
-    <hyperlink ref="F25" r:id="rId117" xr:uid="{E4C74050-943A-4348-9344-B6692C96A745}"/>
-    <hyperlink ref="F32" r:id="rId118" xr:uid="{8176D4E4-9132-4B81-BBAA-7682A6369A8A}"/>
-    <hyperlink ref="F33" r:id="rId119" xr:uid="{BF655D2B-D90F-4CB4-A602-0C3C518CC049}"/>
-    <hyperlink ref="F34" r:id="rId120" xr:uid="{CA051A34-095E-4232-B04F-8E9FF78F8FE5}"/>
-    <hyperlink ref="F35" r:id="rId121" xr:uid="{F5230DC4-5181-4EB6-A3C4-09AFB5DEDCD6}"/>
-    <hyperlink ref="F47" r:id="rId122" xr:uid="{2FEE8DB8-1DBA-4D3F-B942-CDE6B8201DBA}"/>
-    <hyperlink ref="F50" r:id="rId123" xr:uid="{F9A71C84-339F-4332-883A-793A5279F7CF}"/>
-    <hyperlink ref="F51" r:id="rId124" xr:uid="{BF86D58D-72F4-481D-A118-3FAE08817096}"/>
-    <hyperlink ref="F52" r:id="rId125" xr:uid="{4BADF725-C66D-4D78-84F0-A9EE68A26A48}"/>
-    <hyperlink ref="F53" r:id="rId126" xr:uid="{BF05181B-FB72-4F6A-B925-22E06EEBD076}"/>
-    <hyperlink ref="F55" r:id="rId127" xr:uid="{705B1C43-7E31-4BA1-BB6F-E8685A0EE2F0}"/>
-    <hyperlink ref="F61" r:id="rId128" xr:uid="{CCF265E3-CCA9-42AB-9B7F-81CDEFA6EEF8}"/>
-    <hyperlink ref="F66" r:id="rId129" xr:uid="{E1FFC591-19EE-4544-AFA9-924519B5BF99}"/>
-    <hyperlink ref="F73" r:id="rId130" xr:uid="{36E27D57-9C63-402F-8E64-8024AC058ED1}"/>
-    <hyperlink ref="F78" r:id="rId131" xr:uid="{07F18462-9A49-4180-BEE3-0281D972C730}"/>
-    <hyperlink ref="F81" r:id="rId132" xr:uid="{A0D54C38-835C-4D1F-AE02-D99B437C012F}"/>
-    <hyperlink ref="F83" r:id="rId133" xr:uid="{39B94E8F-E2DB-4566-8128-B40B864B986E}"/>
-    <hyperlink ref="F84" r:id="rId134" xr:uid="{6216D95E-A97A-447F-862B-5AAE5D224416}"/>
-    <hyperlink ref="F85" r:id="rId135" xr:uid="{41EA29F7-EE20-454C-B947-A7AF3D7162E4}"/>
-    <hyperlink ref="F86" r:id="rId136" xr:uid="{3A94B2FE-C724-451A-ADCC-C3D72A5FB4EE}"/>
-    <hyperlink ref="F87" r:id="rId137" xr:uid="{60780240-2D2C-4685-BE6A-89203B380568}"/>
-    <hyperlink ref="F89" r:id="rId138" xr:uid="{D45B915A-C954-40DF-A0FF-1152A3B84023}"/>
-    <hyperlink ref="F90" r:id="rId139" xr:uid="{C77F15D2-726D-433F-BAF7-CE4CCD116903}"/>
-    <hyperlink ref="F91" r:id="rId140" xr:uid="{9D25038C-F4D4-4FD0-8160-1AAD13372298}"/>
-    <hyperlink ref="F93" r:id="rId141" xr:uid="{11CCE9AF-DAC5-44EF-9920-589EE9E7863D}"/>
-    <hyperlink ref="F102" r:id="rId142" xr:uid="{D31E20F5-4B75-4041-8DA2-D1FBA96AFB6C}"/>
-    <hyperlink ref="F104" r:id="rId143" xr:uid="{08CF1871-018A-4D45-BBB2-CD5BFCAD5628}"/>
-    <hyperlink ref="F105" r:id="rId144" xr:uid="{26B7E05D-A764-4710-B36A-AD05D2A0DDAA}"/>
-    <hyperlink ref="F106" r:id="rId145" xr:uid="{EFF9E1F9-8DFE-49D8-AA5A-6DD34881E8D5}"/>
-    <hyperlink ref="F108" r:id="rId146" xr:uid="{0FF6572C-698B-49CB-9D39-458AF086C282}"/>
-    <hyperlink ref="F109" r:id="rId147" xr:uid="{3BE7CB94-374E-45F5-9A01-14E192831D5C}"/>
-    <hyperlink ref="F114" r:id="rId148" xr:uid="{3C77CA3E-8C16-4B1F-82CE-3BCB2977324B}"/>
-    <hyperlink ref="F76" r:id="rId149" xr:uid="{68ADB003-7AA3-4AFE-B6F8-DEAF9C96BB13}"/>
-    <hyperlink ref="F70" r:id="rId150" xr:uid="{37D06BD9-FF5F-45E4-B8D7-E515784C5BD9}"/>
+    <hyperlink ref="E31" r:id="rId20" xr:uid="{25EDA559-2CEF-4E44-8A06-E546F2B84006}"/>
+    <hyperlink ref="E36" r:id="rId21" xr:uid="{8FD33C4B-1CE3-46B3-A345-C21880F1752B}"/>
+    <hyperlink ref="E37" r:id="rId22" xr:uid="{93933E02-1ADB-4833-B0BF-E76973463EFD}"/>
+    <hyperlink ref="E38" r:id="rId23" xr:uid="{D4C64ECE-73E4-4CA3-AB45-13D807C4BCD1}"/>
+    <hyperlink ref="E39" r:id="rId24" xr:uid="{726B6699-D227-4F54-9DF6-317184A039DA}"/>
+    <hyperlink ref="E40" r:id="rId25" xr:uid="{79F1D1C5-D2E3-4FB6-8A42-30B6AAEEF86B}"/>
+    <hyperlink ref="E41" r:id="rId26" xr:uid="{20E8E01D-78AA-47AC-9647-41ACA9F319CB}"/>
+    <hyperlink ref="E43" r:id="rId27" xr:uid="{6A1DBB6C-24C8-41BD-A533-0EA7030055CA}"/>
+    <hyperlink ref="E44" r:id="rId28" xr:uid="{38840935-F564-4B2F-AF98-2373338AD887}"/>
+    <hyperlink ref="E45" r:id="rId29" xr:uid="{7D0E3DAE-672A-426E-ACAC-FAE418B4A88B}"/>
+    <hyperlink ref="E46" r:id="rId30" xr:uid="{B9916AA6-CF01-4BC3-BCC9-F57517EFCE1E}"/>
+    <hyperlink ref="E48" r:id="rId31" display="https://www.researchgate.net/profile/Kenneth_David_Strang/publication/318759251_Compressed_school_week_cultural_bias_against_English_Second_Language_student_performance_on_standardized_exams/links/597beb0a0f7e9b8802a94eae/Compressed-school-week-cultural-bias-against-English-Second-Language-student-performance-on-standardized-exams.pdf" xr:uid="{7FB4992C-4B4C-43CD-B296-8FFB935B2BF6}"/>
+    <hyperlink ref="E49" r:id="rId32" xr:uid="{9F240B81-948D-4D36-A688-55516C839E5B}"/>
+    <hyperlink ref="E54" r:id="rId33" xr:uid="{AFB2864A-A3BE-41C4-B7A2-577848D39FDF}"/>
+    <hyperlink ref="E56" r:id="rId34" xr:uid="{55D8ECA8-7BB8-43B4-8508-68F0B8B1327A}"/>
+    <hyperlink ref="E57" r:id="rId35" xr:uid="{403C5BB8-0295-4B17-A4BE-A7B60248A0E6}"/>
+    <hyperlink ref="E58" r:id="rId36" xr:uid="{4FF8993C-AF6D-4835-98AE-76B962E123C7}"/>
+    <hyperlink ref="E59" r:id="rId37" xr:uid="{ABC7321F-2557-486C-814E-68916EB62DAE}"/>
+    <hyperlink ref="E60" r:id="rId38" xr:uid="{0DDA3743-0C6A-4669-904F-B50DB4671549}"/>
+    <hyperlink ref="E62" r:id="rId39" xr:uid="{FBE4A921-F47C-49B4-920A-66482F71D76C}"/>
+    <hyperlink ref="E63" r:id="rId40" xr:uid="{EB5B1EAB-5BAD-4F14-8508-F98623DA2E55}"/>
+    <hyperlink ref="E65" r:id="rId41" xr:uid="{19EDA5A9-D350-4878-8439-07D4C5D87CA9}"/>
+    <hyperlink ref="E67" r:id="rId42" xr:uid="{29CAADCE-6EA2-4A75-A855-EA8C417DFC2E}"/>
+    <hyperlink ref="E68" r:id="rId43" xr:uid="{0FFE9A48-9BF4-450F-8C41-448EA45A1037}"/>
+    <hyperlink ref="E69" r:id="rId44" xr:uid="{7B403720-5732-4579-A81A-460233994424}"/>
+    <hyperlink ref="E71" r:id="rId45" xr:uid="{6E10ACEA-B39A-4D9B-B860-BC22E689266B}"/>
+    <hyperlink ref="E72" r:id="rId46" xr:uid="{B6653391-ACA1-49A5-B4A7-0383B0336B36}"/>
+    <hyperlink ref="E75" r:id="rId47" xr:uid="{B93D594A-EBBD-435A-ABC8-033AA4A45C28}"/>
+    <hyperlink ref="G76" r:id="rId48" xr:uid="{EE0BFC8C-3D01-42C2-BAEB-B237BABF1A69}"/>
+    <hyperlink ref="E77" r:id="rId49" xr:uid="{3F6F9499-A97E-4D52-B3A3-0FC835000504}"/>
+    <hyperlink ref="E79" r:id="rId50" xr:uid="{29055D43-0525-4622-B58C-20DC934FBDC6}"/>
+    <hyperlink ref="E80" r:id="rId51" xr:uid="{9809B794-EB38-4209-AEE7-7CD866741154}"/>
+    <hyperlink ref="E82" r:id="rId52" xr:uid="{CFE5B0D6-A49F-46D0-AE67-5AF70E374F92}"/>
+    <hyperlink ref="E88" r:id="rId53" xr:uid="{E33C5101-8016-4004-97FF-0229DF5D2814}"/>
+    <hyperlink ref="E92" r:id="rId54" location="main" xr:uid="{62C8B0B9-4840-49B2-834E-11D0CF4C253A}"/>
+    <hyperlink ref="E94" r:id="rId55" xr:uid="{3CA66FC6-9EAD-4A9D-B0D5-89C0D376292D}"/>
+    <hyperlink ref="E95" r:id="rId56" xr:uid="{82B11CD5-828F-4A24-AB3F-193982E7E8F8}"/>
+    <hyperlink ref="E96" r:id="rId57" xr:uid="{09D59EDF-991D-4D4A-B2CC-A500EB72581A}"/>
+    <hyperlink ref="E99" r:id="rId58" xr:uid="{7D9732F8-4B86-4CC0-BA46-9476AC4FED46}"/>
+    <hyperlink ref="E100" r:id="rId59" xr:uid="{4237288E-4FBF-4F0F-A678-3D2F910795B5}"/>
+    <hyperlink ref="E101" r:id="rId60" xr:uid="{7E5142FC-179E-40DE-9659-9A2FF9FBE683}"/>
+    <hyperlink ref="E107" r:id="rId61" xr:uid="{7B23BB16-71A0-48CE-805C-BFB42298FBE0}"/>
+    <hyperlink ref="E110" r:id="rId62" xr:uid="{4F277C05-BFBA-449F-8752-0E307436EF8B}"/>
+    <hyperlink ref="E111" r:id="rId63" xr:uid="{1BD26E75-488F-4E14-868C-15F5076003C8}"/>
+    <hyperlink ref="E112" r:id="rId64" xr:uid="{82B04AC4-0EEA-4F80-9B1C-210DE51E94D2}"/>
+    <hyperlink ref="E115" r:id="rId65" xr:uid="{AAA3C322-12A9-4415-922C-74D81FBD97D0}"/>
+    <hyperlink ref="G35" r:id="rId66" xr:uid="{37DEB6BB-AE21-4D65-82EC-6C9DBF9BF72E}"/>
+    <hyperlink ref="G47" r:id="rId67" xr:uid="{9CB66888-A383-4365-8DD1-455302DF0674}"/>
+    <hyperlink ref="G19" r:id="rId68" xr:uid="{711B05F0-8104-4514-A551-999C459B0406}"/>
+    <hyperlink ref="G20" r:id="rId69" xr:uid="{86C3D1CA-AFBE-4DEA-B627-F3EE69FC817E}"/>
+    <hyperlink ref="G23" r:id="rId70" xr:uid="{25A09BFF-36CF-4D51-A291-6A60A992586B}"/>
+    <hyperlink ref="G10" r:id="rId71" xr:uid="{DB27E19D-8146-406B-B6BF-26A5F14B3B99}"/>
+    <hyperlink ref="G33" r:id="rId72" xr:uid="{E07246F3-7066-4F69-A65F-98254F580ED2}"/>
+    <hyperlink ref="G32" r:id="rId73" xr:uid="{897C07DD-A940-4F52-BC65-355F4C7ED66F}"/>
+    <hyperlink ref="G66" r:id="rId74" xr:uid="{E00F78D5-8C8F-4AC0-A5D3-3FB528B3DEDC}"/>
+    <hyperlink ref="G70" r:id="rId75" xr:uid="{A052380E-5C98-42C1-A932-5875FDD6FE6B}"/>
+    <hyperlink ref="G73" r:id="rId76" xr:uid="{D5AD41E6-31BC-4E7C-B124-CA962E91B529}"/>
+    <hyperlink ref="G78" r:id="rId77" xr:uid="{1B103026-3767-4018-A1DF-7926BB7E5E25}"/>
+    <hyperlink ref="E64" r:id="rId78" xr:uid="{6FBC4659-CC58-4CDB-A278-79E1B49004ED}"/>
+    <hyperlink ref="G114" r:id="rId79" xr:uid="{46369FA8-2E83-4232-8E12-11FB6447F57B}"/>
+    <hyperlink ref="G113" r:id="rId80" xr:uid="{0C747466-E2A8-4064-9664-38F8692D95BE}"/>
+    <hyperlink ref="G52" r:id="rId81" xr:uid="{79A57BCB-B8A3-42ED-81D1-697677848967}"/>
+    <hyperlink ref="G50" r:id="rId82" xr:uid="{103E2B00-BE99-4D64-A40E-B74E114EFDDE}"/>
+    <hyperlink ref="G34" r:id="rId83" xr:uid="{CB043E3A-3A12-403C-A0EE-125259BC7972}"/>
+    <hyperlink ref="G6" r:id="rId84" xr:uid="{241256EE-D80C-425A-9E44-65827416D99C}"/>
+    <hyperlink ref="E27" r:id="rId85" xr:uid="{1E13DD51-B7EB-4EFC-A0A9-D847FE9069E7}"/>
+    <hyperlink ref="G55" r:id="rId86" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Impact+of+a+Four-Day+School+Week+on+Student+Discipline+and+Attendance+in+Missouri%3A+A+Quantitative+Study&amp;issn=&amp;date=2021-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Rowden%2C+Angelina&amp;isbn=9798492723514&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{38DBFA6E-C515-4D3D-87CC-444C2A425398}"/>
+    <hyperlink ref="G81" r:id="rId87" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Scheduling+adolescent+achievement%3A+Eighth-graders+and+the+four-day+school+week&amp;issn=&amp;date=2016-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Hegwood%2C+Jessica+Fleming&amp;isbn=978-1-369-48263-8&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{0613F951-D1AE-4EC3-9833-FA8C4694221E}"/>
+    <hyperlink ref="G83" r:id="rId88" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Elementary+Teachers%27+Perceptions+of+Appropriate+Collaborative+Planning+and+Professional+Planning+Time%3A+A+Case+Study&amp;issn=&amp;date=2017-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Wise%2C+Kristi&amp;isbn=978-0-355-10267-3&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{14A9FBBA-105C-4B03-9ABF-4E2F2F55564C}"/>
+    <hyperlink ref="G84" r:id="rId89" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=How+Teachers+Feel+Missouri+School+Schedules+Affect+Teachers+Morale%3A+A+Qualitative+Descriptive+Case+Study&amp;issn=&amp;date=2021-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Smith%2C+Tanya&amp;isbn=979-8-209-99102-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{D4DF9A4B-640B-439E-8775-F74D9F97A2DC}"/>
+    <hyperlink ref="G85" r:id="rId90" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=The+four-day+school+calendar%3A+A+comparative+study+of+student+performance+indicators+in+a+Colorado+school+district&amp;issn=&amp;date=2014-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Reeves%2C+Cheryl+L.&amp;isbn=978-1-303-87204-4&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{5226B787-9144-4A5E-9FBA-10DA9A3B75F6}"/>
+    <hyperlink ref="G87" r:id="rId91" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=The+effect+of+widespread+teacher+furlough+implementation+on+student+performance+on+the+reading%2C+mathematics%2C+and+science+portions+of+the+Hawaiii+State+Assessment&amp;issn=&amp;date=2014-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Lemmer%2C+Bridina+Marie&amp;isbn=978-1-321-05010-3&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{A5E16556-D2D1-4118-90B8-1FEC9124EC80}"/>
+    <hyperlink ref="G89" r:id="rId92" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Explorations+of+Student+and+Parent+Perceptions+of+Changes+in+Traditional+School+Schedule+and+Curriculum+to+Enhance+Competitiveness+with+Charter+Schools&amp;issn=&amp;date=2010-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Kelly%2C+Tiffany+K.&amp;isbn=978-1-124-37958-6&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{A20ED369-9206-4906-B16F-133E337B24F8}"/>
+    <hyperlink ref="G61" r:id="rId93" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Multicase+Exploration+of+Teachers%E2%80%99+Perceptions+of+Experience+of+Working+in+a+4-Day+Work+Week+School+System+Compared+to+a+5-Day+Work+Week+School+System&amp;issn=&amp;date=2020-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Reyes%2C+Lyscelle+M.&amp;isbn=9798698539339&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{19366349-0389-4EB5-BFAA-5FC19CEFC271}"/>
+    <hyperlink ref="G102" r:id="rId94" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=A+COMPARATIVE+CASE+STUDY+OF+THREE+MINNESOTA+SCHOOL+DISTRICTS+EMPLOYING+THE+FOUR-DAY-WEEK+DURING+1982-1983&amp;issn=&amp;date=1985-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=GUSHWA%2C+PRUDENCE+JOANNE&amp;isbn=979-8-205-15586-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{22F43609-39E4-4E93-A3FE-7092A4189348}"/>
+    <hyperlink ref="G91" r:id="rId95" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=A+Quasi-Experimental+Study+Comparing+Work-Life+Balance+and+Turnover+Intentions+Among+Rural+Oklahoma+Classroom+Teachers+Working+Four-Day+and+Five-Day+School+Weeks&amp;issn=&amp;date=2023-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Farber%2C+Misty+Dawn&amp;isbn=9798379420468&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{F99BA589-6518-4F6C-8F80-7D891CE3643F}"/>
+    <hyperlink ref="G93" r:id="rId96" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=The+Four-Day+School+Week+as+a+Path+for+Principal+Attraction+and+Retention%3A+Perceptions+of+Elementary+Principals+in+Missouri&amp;issn=&amp;date=2022-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Weber%2C+Laura+Elizabeth&amp;isbn=9798371990358&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{080115B2-EE11-4BBB-9C85-4C7B4A1AB587}"/>
+    <hyperlink ref="G25" r:id="rId97" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Can+the+4-day+school+week+work%3A+An+analysis+of+the+impact+of+the+4-day+school+week+on+a+rural+Georgia+school+district&amp;issn=&amp;date=2011-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Bell%2C+Jeffrey+L.&amp;isbn=978-1-124-72727-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{6C849674-A5F1-4DB7-97F2-46FD9340B54D}"/>
+    <hyperlink ref="G53" r:id="rId98" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=A+Case+Study+of+the+Influence+of+the+Four-Day+School+Week+on+an+Arizona+School+District&amp;issn=&amp;date=2018-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Savage%2C+Rachel+Marie&amp;isbn=978-0-355-82962-4&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{B6C75ECC-C9F1-43F9-B04E-41908ACC4FFD}"/>
+    <hyperlink ref="G51" r:id="rId99" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Impact+of+a+Four-Day+School+Week+on+Teacher+Preparation&amp;issn=&amp;date=2019-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Schultz%2C+Shawn+C.&amp;isbn=9798662399600&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{0ADED006-B3E9-4FB5-8E8A-C756268CB195}"/>
+    <hyperlink ref="G90" r:id="rId100" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=Students%27+Scores+and+Attendance%3A+A+Study+of+South+Dakota+Schools+with+Four-Day+Schedules&amp;issn=&amp;date=2018-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Dolezal%2C+Dennis+W.&amp;isbn=978-0-355-97001-2&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{1543DFBB-C869-4A54-8C15-B482BC5DB0EA}"/>
+    <hyperlink ref="G105" r:id="rId101" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:book&amp;genre=report&amp;sid=ProQ:ProQ%3Aeric&amp;atitle=&amp;title=Colorado%27s+Alternative+School+Calendar+Program+and+the+Four+Day+Week&amp;issn=&amp;date=1982-01-01&amp;volume=&amp;issue=&amp;spage=1&amp;au=Brubacher%2C+Roy+G.%3BStiverson%2C+C.+L.&amp;isbn=&amp;jtitle=&amp;btitle=Colorado%27s+Alternative+School+Calendar+Program+and+the+Four+Day+Week&amp;rft_id=info:eric/ED214719&amp;rft_id=info:doi/" xr:uid="{6F06FFCC-824A-40D9-A384-F16940E98EDB}"/>
+    <hyperlink ref="G109" r:id="rId102" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:journal&amp;genre=article&amp;sid=ProQ:ProQ%3Aeric&amp;atitle=Changing+the+School+Calendar+to+Effect+Energy+Savings&amp;title=School+Business+Affairs&amp;issn=&amp;date=1980-01-01&amp;volume=46&amp;issue=1&amp;spage=11&amp;au=Webb%2C+L.+Dean%3BAshby%2C+Glenn+H.&amp;isbn=&amp;jtitle=School+Business+Affairs&amp;btitle=&amp;rft_id=info:eric/EJ214271&amp;rft_id=info:doi/" xr:uid="{1DBAFCB4-F00A-416F-88E4-8973143D463B}"/>
+    <hyperlink ref="G98" r:id="rId103" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:ProQuest+Dissertations+%26+Theses+A%26I&amp;atitle=&amp;title=Investigation+of+the+four-day+school+week&amp;issn=&amp;date=2010-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Bronson%2C+Elizabeth+L.&amp;isbn=979-8-209-73276-1&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{5DDB6C57-84FC-4BC3-AB9B-5533118D109F}"/>
+    <hyperlink ref="G12" r:id="rId104" display="https://alliance-uoregon.primo.exlibrisgroup.com/openurl/01ALLIANCE_UO/01ALLIANCE_UO:UO??url_ver=Z39.88-2004&amp;rft_val_fmt=info:ofi/fmt:kev:mtx:dissertation&amp;genre=dissertations&amp;sid=ProQ:Education+Database&amp;atitle=&amp;title=The+four-day+school+week%3A+Teacher+perceptions+in+a+rural%2Fsecondary+setting&amp;issn=&amp;date=2013-01-01&amp;volume=&amp;issue=&amp;spage=&amp;au=Farris%2C+Brandon&amp;isbn=978-1-303-13374-9&amp;jtitle=&amp;btitle=&amp;rft_id=info:eric/&amp;rft_id=info:doi/" xr:uid="{C7A612FE-CED7-4984-B813-1D91DF15C00F}"/>
+    <hyperlink ref="G116" r:id="rId105" xr:uid="{C3FFAE78-7C53-4025-9DF8-CAB3F0011CBB}"/>
+    <hyperlink ref="E2" r:id="rId106" xr:uid="{09C3CA8A-8BC2-4AD9-B08C-84D514554E65}"/>
+    <hyperlink ref="E42" r:id="rId107" xr:uid="{BF57E8F0-8379-4844-A2C0-F3339AC66230}"/>
+    <hyperlink ref="F6" r:id="rId108" xr:uid="{4F06BD45-FC94-4C44-A215-69F3313C6F3F}"/>
+    <hyperlink ref="F10" r:id="rId109" xr:uid="{A13FFFD4-5A08-4BF7-BA9B-D46FA8324C1C}"/>
+    <hyperlink ref="F12" r:id="rId110" xr:uid="{1BF1EA1D-43D8-476D-8BAF-0D9476A35A08}"/>
+    <hyperlink ref="F19" r:id="rId111" xr:uid="{B23139D9-52FE-4A2D-B41C-6AEDA6C1E6BB}"/>
+    <hyperlink ref="F20" r:id="rId112" xr:uid="{945210BB-F866-4ADB-B638-6CA4F832B0A6}"/>
+    <hyperlink ref="F23" r:id="rId113" xr:uid="{08E25523-8C97-448B-96F4-B0C84E945DB7}"/>
+    <hyperlink ref="F25" r:id="rId114" xr:uid="{E4C74050-943A-4348-9344-B6692C96A745}"/>
+    <hyperlink ref="F32" r:id="rId115" xr:uid="{8176D4E4-9132-4B81-BBAA-7682A6369A8A}"/>
+    <hyperlink ref="F33" r:id="rId116" xr:uid="{BF655D2B-D90F-4CB4-A602-0C3C518CC049}"/>
+    <hyperlink ref="F34" r:id="rId117" xr:uid="{CA051A34-095E-4232-B04F-8E9FF78F8FE5}"/>
+    <hyperlink ref="F35" r:id="rId118" xr:uid="{F5230DC4-5181-4EB6-A3C4-09AFB5DEDCD6}"/>
+    <hyperlink ref="F47" r:id="rId119" xr:uid="{2FEE8DB8-1DBA-4D3F-B942-CDE6B8201DBA}"/>
+    <hyperlink ref="F50" r:id="rId120" xr:uid="{F9A71C84-339F-4332-883A-793A5279F7CF}"/>
+    <hyperlink ref="F51" r:id="rId121" xr:uid="{BF86D58D-72F4-481D-A118-3FAE08817096}"/>
+    <hyperlink ref="F52" r:id="rId122" xr:uid="{4BADF725-C66D-4D78-84F0-A9EE68A26A48}"/>
+    <hyperlink ref="F53" r:id="rId123" xr:uid="{BF05181B-FB72-4F6A-B925-22E06EEBD076}"/>
+    <hyperlink ref="F55" r:id="rId124" xr:uid="{705B1C43-7E31-4BA1-BB6F-E8685A0EE2F0}"/>
+    <hyperlink ref="F61" r:id="rId125" xr:uid="{CCF265E3-CCA9-42AB-9B7F-81CDEFA6EEF8}"/>
+    <hyperlink ref="F66" r:id="rId126" xr:uid="{E1FFC591-19EE-4544-AFA9-924519B5BF99}"/>
+    <hyperlink ref="F73" r:id="rId127" xr:uid="{36E27D57-9C63-402F-8E64-8024AC058ED1}"/>
+    <hyperlink ref="F78" r:id="rId128" xr:uid="{07F18462-9A49-4180-BEE3-0281D972C730}"/>
+    <hyperlink ref="F81" r:id="rId129" xr:uid="{A0D54C38-835C-4D1F-AE02-D99B437C012F}"/>
+    <hyperlink ref="F83" r:id="rId130" xr:uid="{39B94E8F-E2DB-4566-8128-B40B864B986E}"/>
+    <hyperlink ref="F84" r:id="rId131" xr:uid="{6216D95E-A97A-447F-862B-5AAE5D224416}"/>
+    <hyperlink ref="F85" r:id="rId132" xr:uid="{41EA29F7-EE20-454C-B947-A7AF3D7162E4}"/>
+    <hyperlink ref="F86" r:id="rId133" xr:uid="{3A94B2FE-C724-451A-ADCC-C3D72A5FB4EE}"/>
+    <hyperlink ref="F87" r:id="rId134" xr:uid="{60780240-2D2C-4685-BE6A-89203B380568}"/>
+    <hyperlink ref="F89" r:id="rId135" xr:uid="{D45B915A-C954-40DF-A0FF-1152A3B84023}"/>
+    <hyperlink ref="F90" r:id="rId136" xr:uid="{C77F15D2-726D-433F-BAF7-CE4CCD116903}"/>
+    <hyperlink ref="F91" r:id="rId137" xr:uid="{9D25038C-F4D4-4FD0-8160-1AAD13372298}"/>
+    <hyperlink ref="F93" r:id="rId138" xr:uid="{11CCE9AF-DAC5-44EF-9920-589EE9E7863D}"/>
+    <hyperlink ref="F102" r:id="rId139" xr:uid="{D31E20F5-4B75-4041-8DA2-D1FBA96AFB6C}"/>
+    <hyperlink ref="F104" r:id="rId140" xr:uid="{08CF1871-018A-4D45-BBB2-CD5BFCAD5628}"/>
+    <hyperlink ref="F105" r:id="rId141" xr:uid="{26B7E05D-A764-4710-B36A-AD05D2A0DDAA}"/>
+    <hyperlink ref="F106" r:id="rId142" xr:uid="{EFF9E1F9-8DFE-49D8-AA5A-6DD34881E8D5}"/>
+    <hyperlink ref="F108" r:id="rId143" xr:uid="{0FF6572C-698B-49CB-9D39-458AF086C282}"/>
+    <hyperlink ref="F109" r:id="rId144" xr:uid="{3BE7CB94-374E-45F5-9A01-14E192831D5C}"/>
+    <hyperlink ref="F114" r:id="rId145" xr:uid="{3C77CA3E-8C16-4B1F-82CE-3BCB2977324B}"/>
+    <hyperlink ref="F76" r:id="rId146" xr:uid="{68ADB003-7AA3-4AFE-B6F8-DEAF9C96BB13}"/>
+    <hyperlink ref="F70" r:id="rId147" xr:uid="{37D06BD9-FF5F-45E4-B8D7-E515784C5BD9}"/>
+    <hyperlink ref="E74" r:id="rId148" xr:uid="{7C613927-3781-4503-BA90-4FFFA86CC5F9}"/>
+    <hyperlink ref="E97" r:id="rId149" xr:uid="{99A8C6DD-2AB1-4125-AB8C-F0143D5C0BB6}"/>
+    <hyperlink ref="E30" r:id="rId150" xr:uid="{D70B88AD-F1F7-4DF4-A2F1-B6FB662309DC}"/>
+    <hyperlink ref="E103" r:id="rId151" display="https://troyuniversity.on.worldcat.org/search/detail/719377305?queryString=ti%3A%28%E2%80%A2%09A%20comparative%20study%20of%20transportation%20costs%20for%20a%20four-day%20school%20week%20and%20a%20five%20day%20school%20week%20for%20Dougherty%20County%20schools%29&amp;databaseList=217%2C283%2C285%2C638&amp;origPageViewName=pages%2Fadvanced-search-page&amp;clusterResults=&amp;groupVariantRecords=&amp;expandSearch=true&amp;translateSearch=false&amp;queryTranslationLanguage=&amp;lang=en&amp;scope=wz%3A475" xr:uid="{988E72D6-7267-4742-83FC-666AF52BCC62}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId151"/>
+  <pageSetup orientation="portrait" r:id="rId152"/>
 </worksheet>
 </file>
</xml_diff>